<commit_message>
Arebic Input field and one field personal address added
</commit_message>
<xml_diff>
--- a/MyInsider/Application/InsiderTrading/Document/Templates/MassUpload/EmployeeMassUploadTemplate.xlsx
+++ b/MyInsider/Application/InsiderTrading/Document/Templates/MassUpload/EmployeeMassUploadTemplate.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D41BCD-306B-4CA7-9E06-DF2C1DEB21B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmpInsider" sheetId="1" r:id="rId1"/>
@@ -23,12 +24,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -52,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -76,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -102,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -133,12 +134,12 @@
 </file>
 
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
       <text>
         <r>
           <rPr>
@@ -162,7 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000002000000}">
       <text>
         <r>
           <rPr>
@@ -191,12 +192,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -220,7 +221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -244,7 +245,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -270,7 +271,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -301,12 +302,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -330,7 +331,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -354,7 +355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -385,12 +386,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -414,7 +415,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -438,7 +439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -462,7 +463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -491,12 +492,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -520,7 +521,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -544,7 +545,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
       <text>
         <r>
           <rPr>
@@ -568,7 +569,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
       <text>
         <r>
           <rPr>
@@ -597,12 +598,12 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -626,7 +627,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -655,12 +656,12 @@
 </file>
 
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -684,7 +685,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
       <text>
         <r>
           <rPr>
@@ -713,12 +714,12 @@
 </file>
 
 <file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
       <text>
         <r>
           <rPr>
@@ -742,7 +743,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000002000000}">
       <text>
         <r>
           <rPr>
@@ -771,12 +772,12 @@
 </file>
 
 <file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
       <text>
         <r>
           <rPr>
@@ -800,7 +801,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000002000000}">
       <text>
         <r>
           <rPr>
@@ -829,7 +830,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="53">
   <si>
     <t>EmployeeSequenceNo</t>
   </si>
@@ -986,11 +987,14 @@
   <si>
     <t>Account Type</t>
   </si>
+  <si>
+    <t>PersonalAddress</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1173,6 +1177,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1208,6 +1229,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1383,11 +1421,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,9 +1454,10 @@
     <col min="22" max="22" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1490,6 +1529,9 @@
       </c>
       <c r="X1" s="6" t="s">
         <v>10</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1500,7 +1542,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1551,11 +1593,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1585,7 +1627,7 @@
     <col min="24" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
@@ -1657,6 +1699,9 @@
       </c>
       <c r="X1" s="6" t="s">
         <v>9</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1666,7 +1711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1751,7 +1796,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1818,7 +1863,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1884,7 +1929,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1934,7 +1979,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1986,7 +2031,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2038,7 +2083,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Revert "Arebic Input field and one field personal address added"
</commit_message>
<xml_diff>
--- a/MyInsider/Application/InsiderTrading/Document/Templates/MassUpload/EmployeeMassUploadTemplate.xlsx
+++ b/MyInsider/Application/InsiderTrading/Document/Templates/MassUpload/EmployeeMassUploadTemplate.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D41BCD-306B-4CA7-9E06-DF2C1DEB21B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="EmpInsider" sheetId="1" r:id="rId1"/>
@@ -24,12 +23,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -103,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -134,12 +133,12 @@
 </file>
 
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -163,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000002000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -192,12 +191,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -221,7 +220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -245,7 +244,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -271,7 +270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -302,12 +301,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -331,7 +330,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -355,7 +354,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -386,12 +385,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -415,7 +414,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -439,7 +438,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -463,7 +462,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -492,12 +491,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -521,7 +520,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -545,7 +544,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -569,7 +568,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -598,12 +597,12 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -627,7 +626,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -656,12 +655,12 @@
 </file>
 
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -685,7 +684,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -714,12 +713,12 @@
 </file>
 
 <file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -743,7 +742,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000002000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -772,12 +771,12 @@
 </file>
 
 <file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -801,7 +800,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000002000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -830,7 +829,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="52">
   <si>
     <t>EmployeeSequenceNo</t>
   </si>
@@ -987,14 +986,11 @@
   <si>
     <t>Account Type</t>
   </si>
-  <si>
-    <t>PersonalAddress</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1177,23 +1173,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1229,23 +1208,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1421,11 +1383,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1454,10 +1416,9 @@
     <col min="22" max="22" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1529,9 +1490,6 @@
       </c>
       <c r="X1" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1542,7 +1500,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1593,11 +1551,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Y1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1627,7 +1585,7 @@
     <col min="24" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
@@ -1699,9 +1657,6 @@
       </c>
       <c r="X1" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1711,7 +1666,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1796,7 +1751,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1863,7 +1818,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1929,7 +1884,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1979,7 +1934,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2031,7 +1986,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2083,7 +2038,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Resolved indiRF massupload issues and committed missing script for IndiaRF
</commit_message>
<xml_diff>
--- a/MyInsider/Application/InsiderTrading/Document/Templates/MassUpload/EmployeeMassUploadTemplate.xlsx
+++ b/MyInsider/Application/InsiderTrading/Document/Templates/MassUpload/EmployeeMassUploadTemplate.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15262D0F-913E-4A82-839F-2782E9A3AE9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmpInsider" sheetId="1" r:id="rId1"/>
@@ -23,12 +24,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -52,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -76,7 +77,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -102,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -133,12 +134,12 @@
 </file>
 
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
       <text>
         <r>
           <rPr>
@@ -162,7 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000002000000}">
       <text>
         <r>
           <rPr>
@@ -191,12 +192,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -220,7 +221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -244,7 +245,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -270,7 +271,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -301,12 +302,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -330,7 +331,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -354,7 +355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -385,12 +386,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -414,7 +415,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -438,7 +439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -462,7 +463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -491,12 +492,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -520,7 +521,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -544,7 +545,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
       <text>
         <r>
           <rPr>
@@ -568,7 +569,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
       <text>
         <r>
           <rPr>
@@ -597,12 +598,12 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -626,7 +627,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -655,12 +656,12 @@
 </file>
 
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -684,7 +685,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
       <text>
         <r>
           <rPr>
@@ -713,12 +714,12 @@
 </file>
 
 <file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
       <text>
         <r>
           <rPr>
@@ -742,7 +743,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000002000000}">
       <text>
         <r>
           <rPr>
@@ -771,12 +772,12 @@
 </file>
 
 <file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
       <text>
         <r>
           <rPr>
@@ -800,7 +801,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000002000000}">
       <text>
         <r>
           <rPr>
@@ -990,7 +991,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1173,6 +1174,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1208,6 +1226,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1383,11 +1418,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,7 +1535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1551,11 +1586,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,11 +1701,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1751,7 +1786,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1818,7 +1853,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1884,11 +1919,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,7 +1969,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1986,7 +2021,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2038,7 +2073,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>